<commit_message>
excel and pickle files generated
</commit_message>
<xml_diff>
--- a/excel_files/tags.xlsx
+++ b/excel_files/tags.xlsx
@@ -14,26 +14,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="291">
   <si>
     <t>dc:creator</t>
   </si>
   <si>
+    <t>owl:imports</t>
+  </si>
+  <si>
+    <t>owl:versioninfo</t>
+  </si>
+  <si>
     <t>dc:date</t>
   </si>
   <si>
+    <t>rdfs:comment</t>
+  </si>
+  <si>
     <t>dc:description</t>
   </si>
   <si>
-    <t>owl:imports</t>
-  </si>
-  <si>
-    <t>owl:versioninfo</t>
-  </si>
-  <si>
-    <t>rdfs:comment</t>
-  </si>
-  <si>
     <t>omv:hascreator</t>
   </si>
   <si>
@@ -64,15 +64,18 @@
     <t>omvmmi:hascontentcreator</t>
   </si>
   <si>
+    <t>dc:title</t>
+  </si>
+  <si>
     <t>omvmmi:hasresourcetype</t>
   </si>
   <si>
-    <t>dc:title</t>
-  </si>
-  <si>
     <t>omv:usedontologyengineeringtool</t>
   </si>
   <si>
+    <t>rdfs:label</t>
+  </si>
+  <si>
     <t>omvmmi:shortnameuri</t>
   </si>
   <si>
@@ -91,124 +94,160 @@
     <t>omvmmi:origvocmanager</t>
   </si>
   <si>
+    <t>vann:preferrednamespaceprefix</t>
+  </si>
+  <si>
     <t>omvmmi:contactrole</t>
   </si>
   <si>
-    <t>rdfs:label</t>
+    <t>vann:preferrednamespaceuri</t>
   </si>
   <si>
     <t>omvmmi:contact</t>
   </si>
   <si>
+    <t>owl:versioniri</t>
+  </si>
+  <si>
+    <t>dcterms:modified</t>
+  </si>
+  <si>
+    <t>foaf:homepage</t>
+  </si>
+  <si>
+    <t>rdf:type</t>
+  </si>
+  <si>
+    <t>dcterms:created</t>
+  </si>
+  <si>
+    <t>dcterms:title</t>
+  </si>
+  <si>
+    <t>dcterms:type</t>
+  </si>
+  <si>
+    <t>dcterms:status</t>
+  </si>
+  <si>
+    <t>dcterms:partof</t>
+  </si>
+  <si>
+    <t>dc:source</t>
+  </si>
+  <si>
+    <t>dc:subject</t>
+  </si>
+  <si>
     <t>omv:documentation</t>
   </si>
   <si>
-    <t>dc:source</t>
-  </si>
-  <si>
-    <t>owl:versioniri</t>
-  </si>
-  <si>
-    <t>dc:subject</t>
+    <t>dcterms:publisher</t>
+  </si>
+  <si>
+    <t>dcterms:description</t>
   </si>
   <si>
     <t>omvmmi:origvocuri</t>
   </si>
   <si>
+    <t>oboinowl:default-namespace</t>
+  </si>
+  <si>
+    <t>oboinowl:hasoboformatversion</t>
+  </si>
+  <si>
+    <t>dc:format</t>
+  </si>
+  <si>
     <t>omv:reference</t>
   </si>
   <si>
-    <t>dc:format</t>
-  </si>
-  <si>
     <t>dc:publisher</t>
   </si>
   <si>
+    <t>dc:rights</t>
+  </si>
+  <si>
+    <t>oboinowl:saved-by</t>
+  </si>
+  <si>
+    <t>oboinowl:date</t>
+  </si>
+  <si>
+    <t>oboinowl:auto-generated-by</t>
+  </si>
+  <si>
     <t>omvmmi:origvocdocumentationuri</t>
   </si>
   <si>
     <t>omvmmi:creditcitation</t>
   </si>
   <si>
-    <t>oboinowl:hasoboformatversion</t>
-  </si>
-  <si>
-    <t>oboinowl:default-namespace</t>
-  </si>
-  <si>
     <t>omvmmi:origvocdescriptivename</t>
   </si>
   <si>
-    <t>oboinowl:saved-by</t>
-  </si>
-  <si>
-    <t>dc:rights</t>
+    <t>rdfs:seealso</t>
+  </si>
+  <si>
+    <t>owl:priorversion</t>
+  </si>
+  <si>
+    <t>dc:license</t>
   </si>
   <si>
     <t>omvmmi:origvocsyntaxformat</t>
   </si>
   <si>
-    <t>oboinowl:date</t>
-  </si>
-  <si>
-    <t>owl:priorversion</t>
-  </si>
-  <si>
-    <t>oboinowl:auto-generated-by</t>
+    <t>cc:license</t>
   </si>
   <si>
     <t>protege:defaultlanguage</t>
   </si>
   <si>
-    <t>dc:license</t>
-  </si>
-  <si>
-    <t>rdfs:seealso</t>
+    <t>dc:language</t>
+  </si>
+  <si>
+    <t>swivt:creationdate</t>
   </si>
   <si>
     <t>omvmmi:origvockeywords</t>
   </si>
   <si>
-    <t>dc:language</t>
-  </si>
-  <si>
-    <t>cc:license</t>
-  </si>
-  <si>
-    <t>vann:preferrednamespaceprefix</t>
+    <t>rdfs:isdefinedby</t>
   </si>
   <si>
     <t>omvmmi:origvocversionid</t>
   </si>
   <si>
-    <t>vann:preferrednamespaceuri</t>
-  </si>
-  <si>
-    <t>rdfs:isdefinedby</t>
+    <t>dc:identifier</t>
+  </si>
+  <si>
+    <t>owl:ontology</t>
   </si>
   <si>
     <t>core:changenote</t>
   </si>
   <si>
-    <t>owl:ontology</t>
-  </si>
-  <si>
     <t>dc:issued</t>
   </si>
   <si>
-    <t>dc:identifier</t>
+    <t>dc:modified</t>
+  </si>
+  <si>
+    <t>obo:iao_0000116</t>
   </si>
   <si>
     <t>oboinowl:savedby</t>
   </si>
   <si>
-    <t>dcterms:modified</t>
-  </si>
-  <si>
-    <t>foaf:homepage</t>
-  </si>
-  <si>
-    <t>obo:iao_0000116</t>
+    <t>terms:modified</t>
+  </si>
+  <si>
+    <t>foaf:person</t>
+  </si>
+  <si>
+    <t>dcterms:creator</t>
   </si>
   <si>
     <t>oboinowl:hassubset</t>
@@ -217,85 +256,145 @@
     <t>cpannotationschema:hasintent</t>
   </si>
   <si>
+    <t>dcterms:license</t>
+  </si>
+  <si>
+    <t>vaem:revisionnumber</t>
+  </si>
+  <si>
+    <t>vaem:lastupdated</t>
+  </si>
+  <si>
+    <t>terms:creator</t>
+  </si>
+  <si>
+    <t>foaf:mbox</t>
+  </si>
+  <si>
+    <t>vaem:hasdisciplinescope</t>
+  </si>
+  <si>
     <t>oboinowl:hasdate</t>
   </si>
   <si>
+    <t>vaem:hasaspectscope</t>
+  </si>
+  <si>
+    <t>vaem:usesnonimportedresource</t>
+  </si>
+  <si>
     <t>oboinowl:hasdefaultnamespace</t>
   </si>
   <si>
-    <t>terms:modified</t>
-  </si>
-  <si>
-    <t>dc:modified</t>
-  </si>
-  <si>
-    <t>foaf:mbox</t>
+    <t>vaem:datecreated</t>
+  </si>
+  <si>
+    <t>terms:title</t>
+  </si>
+  <si>
+    <t>vaem:hasdomainscope</t>
+  </si>
+  <si>
+    <t>vaem:hasrole</t>
+  </si>
+  <si>
+    <t>cpannotationschema:hasconsequences</t>
+  </si>
+  <si>
+    <t>cpannotationschema:coversrequirements</t>
+  </si>
+  <si>
+    <t>voag:haslicensetype</t>
+  </si>
+  <si>
+    <t>voag:withattributionto</t>
+  </si>
+  <si>
+    <t>vaem:namespace</t>
+  </si>
+  <si>
+    <t>foaf:name</t>
+  </si>
+  <si>
+    <t>oboinowl:namespaceidrule</t>
+  </si>
+  <si>
+    <t>vaem:description</t>
+  </si>
+  <si>
+    <t>vaem:specificity</t>
   </si>
   <si>
     <t>obo_annot:createddate</t>
   </si>
   <si>
+    <t>skos:preflabel</t>
+  </si>
+  <si>
     <t>obo_annot:modifieddate</t>
   </si>
   <si>
-    <t>skos:preflabel</t>
+    <t>ns0:defaultlanguage</t>
+  </si>
+  <si>
+    <t>cpannotationschema:scenarios</t>
+  </si>
+  <si>
+    <t>cpannotationschema:extractedfrom</t>
   </si>
   <si>
     <t>terms:identifier</t>
   </si>
   <si>
-    <t>ns0:defaultlanguage</t>
-  </si>
-  <si>
-    <t>cpannotationschema:scenarios</t>
-  </si>
-  <si>
-    <t>cpannotationschema:hasconsequences</t>
+    <t>vaem:namespaceprefix</t>
+  </si>
+  <si>
+    <t>skos:altlabel</t>
+  </si>
+  <si>
+    <t>vaem:acronym</t>
+  </si>
+  <si>
+    <t>foaf:page</t>
+  </si>
+  <si>
+    <t>dct:creator</t>
+  </si>
+  <si>
+    <t>voag:hascatalogentry</t>
+  </si>
+  <si>
+    <t>terms:description</t>
   </si>
   <si>
     <t>core:editorialnote</t>
   </si>
   <si>
-    <t>cpannotationschema:coversrequirements</t>
-  </si>
-  <si>
-    <t>skos:altlabel</t>
-  </si>
-  <si>
-    <t>dcterms:creator</t>
-  </si>
-  <si>
-    <t>terms:creator</t>
+    <t>oboinowl:remark</t>
+  </si>
+  <si>
+    <t>cpannotationschema:hasauthor</t>
+  </si>
+  <si>
+    <t>foaf:maker</t>
+  </si>
+  <si>
+    <t>dcterms:issued</t>
+  </si>
+  <si>
+    <t>terms:contributor</t>
+  </si>
+  <si>
+    <t>oboinowl:treat-xrefs-as-equivalent</t>
   </si>
   <si>
     <t>core:definition</t>
   </si>
   <si>
-    <t>terms:title</t>
-  </si>
-  <si>
-    <t>cpannotationschema:extractedfrom</t>
-  </si>
-  <si>
-    <t>foaf:person</t>
-  </si>
-  <si>
-    <t>oboinowl:remark</t>
-  </si>
-  <si>
-    <t>foaf:page</t>
-  </si>
-  <si>
-    <t>foaf:name</t>
-  </si>
-  <si>
-    <t>dcterms:issued</t>
-  </si>
-  <si>
-    <t>oboinowl:namespaceidrule</t>
-  </si>
-  <si>
-    <t>dct:creator</t>
+    <t>terms:license</t>
+  </si>
+  <si>
+    <t>terms:rights</t>
   </si>
   <si>
     <t>skos:definition</t>
@@ -304,64 +403,73 @@
     <t>cpannotationschema:relatedcps</t>
   </si>
   <si>
-    <t>terms:license</t>
-  </si>
-  <si>
-    <t>dcterms:license</t>
+    <t>foaf:organization</t>
+  </si>
+  <si>
+    <t>owl:incompatiblewith</t>
+  </si>
+  <si>
+    <t>oboinowl:treat-xrefs-as-is_a</t>
   </si>
   <si>
     <t>j.0:defaultlanguage</t>
   </si>
   <si>
-    <t>cpannotationschema:hasauthor</t>
-  </si>
-  <si>
-    <t>dcterms:description</t>
-  </si>
-  <si>
-    <t>terms:contributor</t>
+    <t>terms:issued</t>
+  </si>
+  <si>
+    <t>dct:contributor</t>
+  </si>
+  <si>
+    <t>dct:issued</t>
+  </si>
+  <si>
+    <t>dct:created</t>
   </si>
   <si>
     <t>dc:coverage</t>
   </si>
   <si>
+    <t>dc:created</t>
+  </si>
+  <si>
     <t>obo_annot:pendingactionnote</t>
   </si>
   <si>
+    <t>dct:modified</t>
+  </si>
+  <si>
     <t>oboinowl:format-version</t>
   </si>
   <si>
-    <t>oboinowl:treat-xrefs-as-equivalent</t>
+    <t>rdf:description</t>
+  </si>
+  <si>
+    <t>dct:description</t>
+  </si>
+  <si>
+    <t>dct:date</t>
   </si>
   <si>
     <t>oboinowl:subset</t>
   </si>
   <si>
-    <t>terms:rights</t>
-  </si>
-  <si>
-    <t>dct:description</t>
-  </si>
-  <si>
-    <t>owl:incompatiblewith</t>
-  </si>
-  <si>
-    <t>dct:date</t>
-  </si>
-  <si>
-    <t>dcterms:created</t>
-  </si>
-  <si>
-    <t>oboinowl:treat-xrefs-as-is_a</t>
+    <t>vaem:intent</t>
   </si>
   <si>
     <t>doap:version</t>
   </si>
   <si>
-    <t>terms:description</t>
-  </si>
-  <si>
-    <t>dct:contributor</t>
+    <t>ns:license</t>
+  </si>
+  <si>
+    <t>nemo_annot:created_date</t>
+  </si>
+  <si>
+    <t>owl:annotationproperty</t>
+  </si>
+  <si>
+    <t>dct:license</t>
   </si>
   <si>
     <t>oboinowl:treat-xrefs-as-genus-differentia</t>
@@ -370,7 +478,16 @@
     <t>obo:idspace</t>
   </si>
   <si>
-    <t>foaf:maker</t>
+    <t>dcterms:subject</t>
+  </si>
+  <si>
+    <t>nemo_annot:curator</t>
+  </si>
+  <si>
+    <t>dcterms:identifier</t>
+  </si>
+  <si>
+    <t>oboinowl:treat-xrefs-as-reverse-genus-differentia</t>
   </si>
   <si>
     <t>dcterms:contributor</t>
@@ -379,364 +496,394 @@
     <t>obo:default-relationship-id-prefix</t>
   </si>
   <si>
-    <t>dcterms:publisher</t>
+    <t>nemo_annot:pref_label</t>
+  </si>
+  <si>
+    <t>doap:svnrepository</t>
+  </si>
+  <si>
+    <t>rdfs:range</t>
+  </si>
+  <si>
+    <t>dc11:date</t>
+  </si>
+  <si>
+    <t>nemo_annot:synonym</t>
+  </si>
+  <si>
+    <t>dct:title</t>
+  </si>
+  <si>
+    <t>oboinowl:treat-xrefs-as-has-subclass</t>
+  </si>
+  <si>
+    <t>terms:publisher</t>
+  </si>
+  <si>
+    <t>dcat:landingpage</t>
+  </si>
+  <si>
+    <t>dc11:created</t>
+  </si>
+  <si>
+    <t>dc11:publisher</t>
+  </si>
+  <si>
+    <t>obo:format-version</t>
+  </si>
+  <si>
+    <t>doap:mailing-list</t>
+  </si>
+  <si>
+    <t>terms:isreferencedby</t>
+  </si>
+  <si>
+    <t>owl:backwardcompatiblewith</t>
+  </si>
+  <si>
+    <t>prism:doi</t>
+  </si>
+  <si>
+    <t>obo:date</t>
+  </si>
+  <si>
+    <t>doap:gitrepository</t>
+  </si>
+  <si>
+    <t>doap:bug-database</t>
+  </si>
+  <si>
+    <t>vaem:hascatalogentry</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>dc11:creator</t>
+  </si>
+  <si>
+    <t>pav:version</t>
+  </si>
+  <si>
+    <t>efo:creator</t>
+  </si>
+  <si>
+    <t>nemo_annot:modified_date</t>
+  </si>
+  <si>
+    <t>owl:deprecated</t>
+  </si>
+  <si>
+    <t>obo:is_metadata_tag</t>
+  </si>
+  <si>
+    <t>elements:creator</t>
+  </si>
+  <si>
+    <t>j.0:historynote</t>
+  </si>
+  <si>
+    <t>rdf:comment</t>
+  </si>
+  <si>
+    <t>voaf:classnumber</t>
+  </si>
+  <si>
+    <t>j.0:definition</t>
+  </si>
+  <si>
+    <t>foaf:mbox_sha1sum</t>
+  </si>
+  <si>
+    <t>smw:exportdate</t>
+  </si>
+  <si>
+    <t>obo:iao_0000412</t>
+  </si>
+  <si>
+    <t>owl:datatypeproperty</t>
+  </si>
+  <si>
+    <t>void:databrowse</t>
+  </si>
+  <si>
+    <t>dc:right</t>
+  </si>
+  <si>
+    <t>b807e4-4286-46f3-89f6-f67df1657fdc:efo_0000009</t>
+  </si>
+  <si>
+    <t>dct:rights</t>
+  </si>
+  <si>
+    <t>cpannotationschema:hascomponent</t>
+  </si>
+  <si>
+    <t>asthma:defaultlanguage</t>
+  </si>
+  <si>
+    <t>dcterms:isrequiredby</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>dce:date</t>
+  </si>
+  <si>
+    <t>voaf:relieson</t>
+  </si>
+  <si>
+    <t>contributing_author</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>dcat:downloadurl</t>
+  </si>
+  <si>
+    <t>patterns:createdby</t>
+  </si>
+  <si>
+    <t>dcterms:isreferencedby</t>
+  </si>
+  <si>
+    <t>primary_author_and_curator</t>
+  </si>
+  <si>
+    <t>oboinowl:pairwise-disjoint</t>
+  </si>
+  <si>
+    <t>owl:objectproperty</t>
+  </si>
+  <si>
+    <t>oboother:idspace</t>
+  </si>
+  <si>
+    <t>oboinowl:subsetdef</t>
+  </si>
+  <si>
+    <t>j.1:defaultlanguage</t>
+  </si>
+  <si>
+    <t>omvmmi:origvoclastmodified</t>
+  </si>
+  <si>
+    <t>next_id</t>
+  </si>
+  <si>
+    <t>wob:rdfdocument</t>
+  </si>
+  <si>
+    <t>terms:date</t>
+  </si>
+  <si>
+    <t>vs:term_status</t>
+  </si>
+  <si>
+    <t>webprotege:revision</t>
   </si>
   <si>
     <t>core:historynote</t>
   </si>
   <si>
-    <t>dct:title</t>
-  </si>
-  <si>
-    <t>dcterms:title</t>
-  </si>
-  <si>
-    <t>rdf:description</t>
-  </si>
-  <si>
-    <t>dcat:landingpage</t>
-  </si>
-  <si>
-    <t>obo:format-version</t>
-  </si>
-  <si>
-    <t>owl:backwardcompatiblewith</t>
-  </si>
-  <si>
-    <t>prism:doi</t>
-  </si>
-  <si>
-    <t>obo:date</t>
-  </si>
-  <si>
-    <t>dcterms:subject</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>terms:issued</t>
-  </si>
-  <si>
-    <t>pav:version</t>
-  </si>
-  <si>
-    <t>efo:creator</t>
-  </si>
-  <si>
-    <t>nemo_annot:created_date</t>
-  </si>
-  <si>
-    <t>owl:deprecated</t>
-  </si>
-  <si>
-    <t>obo:is_metadata_tag</t>
-  </si>
-  <si>
-    <t>foaf:mbox_sha1sum</t>
+    <t>chmo:has_format-version</t>
+  </si>
+  <si>
+    <t>cc:licence</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>cpannotationschema:isspecializationof</t>
+  </si>
+  <si>
+    <t>voaf:propertynumber</t>
+  </si>
+  <si>
+    <t>dcterms:rights</t>
+  </si>
+  <si>
+    <t>prov:has_provenance</t>
+  </si>
+  <si>
+    <t>specializationof</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>wasrevisionof</t>
+  </si>
+  <si>
+    <t>edamontology1:next_id</t>
+  </si>
+  <si>
+    <t>oboinowl:hasversion</t>
+  </si>
+  <si>
+    <t>rdfs:domain</t>
+  </si>
+  <si>
+    <t>j.0:editorialnote</t>
+  </si>
+  <si>
+    <t>foaf:primarytopic</t>
+  </si>
+  <si>
+    <t>dct:publisher</t>
+  </si>
+  <si>
+    <t>skos:historynote</t>
+  </si>
+  <si>
+    <t>dct:available</t>
+  </si>
+  <si>
+    <t>obo:remark</t>
+  </si>
+  <si>
+    <t>voaf:metadatavoc</t>
+  </si>
+  <si>
+    <t>dcterms:format</t>
+  </si>
+  <si>
+    <t>foaf:isprimarytopicof</t>
+  </si>
+  <si>
+    <t>obo:comment</t>
+  </si>
+  <si>
+    <t>oboother:default-relationship-id-prefix</t>
+  </si>
+  <si>
+    <t>dcterms:language</t>
+  </si>
+  <si>
+    <t>meta:bookmark</t>
   </si>
   <si>
     <t>dct:source</t>
   </si>
   <si>
-    <t>j.0:historynote</t>
-  </si>
-  <si>
-    <t>rdf:comment</t>
-  </si>
-  <si>
-    <t>j.15:defaultlanguage</t>
+    <t>relationship:idspace</t>
+  </si>
+  <si>
+    <t>tool</t>
+  </si>
+  <si>
+    <t>void:datadump</t>
+  </si>
+  <si>
+    <t>owl:class</t>
+  </si>
+  <si>
+    <t>oboother:remark</t>
+  </si>
+  <si>
+    <t>dce:creator</t>
+  </si>
+  <si>
+    <t>j.0:organization</t>
+  </si>
+  <si>
+    <t>technical_support</t>
+  </si>
+  <si>
+    <t>cpannotationschema:hasunittest</t>
+  </si>
+  <si>
+    <t>oboinowl:comment</t>
+  </si>
+  <si>
+    <t>voaf:specializes</t>
+  </si>
+  <si>
+    <t>dce:subject</t>
+  </si>
+  <si>
+    <t>dcterms:lastmodified</t>
+  </si>
+  <si>
+    <t>obo:iao_0000117</t>
+  </si>
+  <si>
+    <t>acetext:acetext</t>
+  </si>
+  <si>
+    <t>dct:hasformat</t>
+  </si>
+  <si>
+    <t>owl:namedindividual</t>
+  </si>
+  <si>
+    <t>j.0:imports</t>
+  </si>
+  <si>
+    <t>rdf:property</t>
+  </si>
+  <si>
+    <t>j.0:license</t>
+  </si>
+  <si>
+    <t>doc:version</t>
+  </si>
+  <si>
+    <t>ns0:license</t>
+  </si>
+  <si>
+    <t>owl:unionof</t>
+  </si>
+  <si>
+    <t>terms:created</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>cito:citesasauthority</t>
+  </si>
+  <si>
+    <t>ontoneo:ontoneo_1000000</t>
+  </si>
+  <si>
+    <t>oboinowl:next-id</t>
+  </si>
+  <si>
+    <t>birn_annot:curationstatus</t>
+  </si>
+  <si>
+    <t>dc:type</t>
+  </si>
+  <si>
+    <t>rdfs:subclassof</t>
+  </si>
+  <si>
+    <t>asthma:creator</t>
+  </si>
+  <si>
+    <t>spin:imports</t>
+  </si>
+  <si>
+    <t>oboinowl:data-version</t>
   </si>
   <si>
     <t>oboother:date</t>
   </si>
   <si>
-    <t>oboother:idspace</t>
-  </si>
-  <si>
-    <t>j.0:definition</t>
-  </si>
-  <si>
-    <t>wasrevisionof</t>
-  </si>
-  <si>
-    <t>dct:license</t>
-  </si>
-  <si>
-    <t>smw:exportdate</t>
-  </si>
-  <si>
-    <t>obo:iao_0000412</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>nemo_annot:curator</t>
-  </si>
-  <si>
-    <t>void:databrowse</t>
-  </si>
-  <si>
-    <t>j.14:modifieddate</t>
-  </si>
-  <si>
-    <t>b807e4-4286-46f3-89f6-f67df1657fdc:efo_0000009</t>
-  </si>
-  <si>
-    <t>rdf:type</t>
-  </si>
-  <si>
-    <t>cpannotationschema:hascomponent</t>
-  </si>
-  <si>
-    <t>dcterms:identifier</t>
-  </si>
-  <si>
-    <t>asthma:defaultlanguage</t>
-  </si>
-  <si>
-    <t>oboinowl:treat-xrefs-as-reverse-genus-differentia</t>
-  </si>
-  <si>
-    <t>next_id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>oboinowl:rgdformat-version</t>
-  </si>
-  <si>
-    <t>owl:ontologyiri</t>
-  </si>
-  <si>
-    <t>j.18:changenote</t>
-  </si>
-  <si>
-    <t>dcat:downloadurl</t>
-  </si>
-  <si>
-    <t>nemo_annot:pref_label</t>
-  </si>
-  <si>
-    <t>foaf:isprimarytopicof</t>
-  </si>
-  <si>
-    <t>creator</t>
-  </si>
-  <si>
-    <t>dct:created</t>
-  </si>
-  <si>
-    <t>patterns:createdby</t>
-  </si>
-  <si>
-    <t>dc:created</t>
-  </si>
-  <si>
-    <t>acetext:acetext</t>
-  </si>
-  <si>
-    <t>obo:comment</t>
-  </si>
-  <si>
-    <t>oboinowl:subsetdef</t>
-  </si>
-  <si>
-    <t>j.1:defaultlanguage</t>
-  </si>
-  <si>
-    <t>nemo_annot:modified_date</t>
-  </si>
-  <si>
-    <t>omvmmi:origvoclastmodified</t>
-  </si>
-  <si>
-    <t>j.18:historynote</t>
-  </si>
-  <si>
-    <t>wob:rdfdocument</t>
-  </si>
-  <si>
-    <t>contributing_author</t>
-  </si>
-  <si>
-    <t>nemo_annot:synonym</t>
-  </si>
-  <si>
-    <t>meta:bookmark</t>
-  </si>
-  <si>
-    <t>j.3:curationstatus</t>
-  </si>
-  <si>
-    <t>cc:licence</t>
-  </si>
-  <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>cpannotationschema:isspecializationof</t>
-  </si>
-  <si>
-    <t>terms:publisher</t>
-  </si>
-  <si>
-    <t>dcterms:rights</t>
-  </si>
-  <si>
-    <t>prov:has_provenance</t>
-  </si>
-  <si>
-    <t>dcterms:bibliographiccitation</t>
-  </si>
-  <si>
-    <t>specializationof</t>
-  </si>
-  <si>
-    <t>doap:gitrepository</t>
-  </si>
-  <si>
-    <t>dct:issued</t>
-  </si>
-  <si>
-    <t>edamontology1:next_id</t>
-  </si>
-  <si>
-    <t>oboinowl:hasversion</t>
-  </si>
-  <si>
-    <t>doap:svnrepository</t>
-  </si>
-  <si>
-    <t>j.0:editorialnote</t>
-  </si>
-  <si>
-    <t>foaf:primarytopic</t>
-  </si>
-  <si>
-    <t>skos:historynote</t>
-  </si>
-  <si>
-    <t>terms:date</t>
-  </si>
-  <si>
-    <t>obo:remark</t>
-  </si>
-  <si>
-    <t>doap:mailing-list</t>
-  </si>
-  <si>
-    <t>dcterms:format</t>
-  </si>
-  <si>
-    <t>foaf:organization</t>
-  </si>
-  <si>
-    <t>oboother:default-relationship-id-prefix</t>
-  </si>
-  <si>
-    <t>j.18:editorialnote</t>
-  </si>
-  <si>
-    <t>relationship:idspace</t>
-  </si>
-  <si>
-    <t>tool</t>
-  </si>
-  <si>
-    <t>void:datadump</t>
-  </si>
-  <si>
-    <t>oboother:remark</t>
-  </si>
-  <si>
-    <t>dce:creator</t>
-  </si>
-  <si>
-    <t>technical_support</t>
-  </si>
-  <si>
-    <t>primary_author_and_curator</t>
-  </si>
-  <si>
-    <t>cpannotationschema:hasunittest</t>
-  </si>
-  <si>
-    <t>oboinowl:comment</t>
-  </si>
-  <si>
-    <t>oboinowl:treat-xrefs-as-has-subclass</t>
-  </si>
-  <si>
-    <t>doc:version</t>
-  </si>
-  <si>
-    <t>dce:subject</t>
-  </si>
-  <si>
-    <t>chmo:has_format-version</t>
-  </si>
-  <si>
-    <t>j.14:pendingactionnote</t>
-  </si>
-  <si>
-    <t>dct:hasformat</t>
-  </si>
-  <si>
-    <t>dcterms:language</t>
-  </si>
-  <si>
-    <t>dce:date</t>
-  </si>
-  <si>
-    <t>j.0:imports</t>
-  </si>
-  <si>
-    <t>j.14:createddate</t>
-  </si>
-  <si>
-    <t>ns0:license</t>
-  </si>
-  <si>
-    <t>doap:bug-database</t>
-  </si>
-  <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>ontoneo:ontoneo_1000000</t>
-  </si>
-  <si>
-    <t>dc:right</t>
-  </si>
-  <si>
-    <t>j.18:definition</t>
-  </si>
-  <si>
-    <t>birn_annot:curationstatus</t>
-  </si>
-  <si>
-    <t>asthma:creator</t>
-  </si>
-  <si>
-    <t>oboinowl:data-version</t>
-  </si>
-  <si>
-    <t>terms:isreferencedby</t>
-  </si>
-  <si>
-    <t>ns:license</t>
-  </si>
-  <si>
     <t>uri</t>
   </si>
   <si>
     <t>oboinowl:synonymtypedef</t>
   </si>
   <si>
-    <t>terms:created</t>
+    <t>oboinowl:default-relationship-id-prefix</t>
   </si>
   <si>
     <t>oboinowl:property-value</t>
@@ -1071,7 +1218,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:B243"/>
+  <dimension ref="A2:B292"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1082,7 +1229,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>448</v>
+        <v>564</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1090,7 +1237,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>352</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1098,7 +1245,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>338</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1106,7 +1253,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>333</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1114,7 +1261,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>299</v>
+        <v>361</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1122,7 +1269,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>275</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1130,7 +1277,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1138,7 +1285,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1146,7 +1293,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1154,7 +1301,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1162,7 +1309,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1170,7 +1317,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1178,7 +1325,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1186,7 +1333,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1194,7 +1341,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>230</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1202,7 +1349,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1210,7 +1357,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1218,7 +1365,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>163</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1226,7 +1373,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1234,7 +1381,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1242,7 +1389,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1250,7 +1397,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>128</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1258,7 +1405,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>111</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1266,7 +1413,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1274,7 +1421,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1282,7 +1429,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1290,7 +1437,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1298,7 +1445,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1306,7 +1453,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>76</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1314,7 +1461,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>75</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1322,7 +1469,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>72</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1330,7 +1477,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>66</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1338,7 +1485,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>60</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1346,7 +1493,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>49</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1354,7 +1501,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>48</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1362,7 +1509,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>46</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1370,7 +1517,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>40</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1378,7 +1525,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>39</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1386,7 +1533,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>37</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1394,7 +1541,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1402,7 +1549,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>36</v>
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1410,7 +1557,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>33</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1418,7 +1565,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>32</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1426,7 +1573,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1434,7 +1581,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>30</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1442,7 +1589,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>29</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1450,7 +1597,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>28</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1458,7 +1605,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1466,7 +1613,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>25</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1474,7 +1621,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -1482,7 +1629,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>23</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -1490,7 +1637,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -1498,7 +1645,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -1506,7 +1653,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -1514,7 +1661,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>16</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -1522,7 +1669,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>15</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -1530,7 +1677,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -1538,7 +1685,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -1546,7 +1693,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -1554,7 +1701,7 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -1562,7 +1709,7 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -1570,7 +1717,7 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>10</v>
+        <v>29</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -1578,7 +1725,7 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>10</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1586,7 +1733,7 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1594,7 +1741,7 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -1602,7 +1749,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -1610,7 +1757,7 @@
         <v>66</v>
       </c>
       <c r="B68">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -1618,7 +1765,7 @@
         <v>67</v>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -1626,7 +1773,7 @@
         <v>68</v>
       </c>
       <c r="B70">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -1634,7 +1781,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1642,7 +1789,7 @@
         <v>70</v>
       </c>
       <c r="B72">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1650,7 +1797,7 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1658,7 +1805,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -1666,7 +1813,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -1674,7 +1821,7 @@
         <v>74</v>
       </c>
       <c r="B76">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1682,7 +1829,7 @@
         <v>75</v>
       </c>
       <c r="B77">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1690,7 +1837,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1698,7 +1845,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1706,7 +1853,7 @@
         <v>78</v>
       </c>
       <c r="B80">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1714,7 +1861,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1722,7 +1869,7 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1730,7 +1877,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1738,7 +1885,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1746,7 +1893,7 @@
         <v>83</v>
       </c>
       <c r="B85">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1754,7 +1901,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1762,7 +1909,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1770,7 +1917,7 @@
         <v>86</v>
       </c>
       <c r="B88">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1778,7 +1925,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1786,7 +1933,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1794,7 +1941,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1802,7 +1949,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1810,7 +1957,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1818,7 +1965,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1826,7 +1973,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1834,7 +1981,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1842,7 +1989,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1850,7 +1997,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1858,7 +2005,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1866,7 +2013,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1874,7 +2021,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -1882,7 +2029,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -1890,7 +2037,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -1898,7 +2045,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -1906,7 +2053,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -1914,7 +2061,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1922,7 +2069,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1930,7 +2077,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1938,7 +2085,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1946,7 +2093,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1954,7 +2101,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1962,7 +2109,7 @@
         <v>110</v>
       </c>
       <c r="B112">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -1970,7 +2117,7 @@
         <v>111</v>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -1978,7 +2125,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -1986,7 +2133,7 @@
         <v>113</v>
       </c>
       <c r="B115">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -1994,7 +2141,7 @@
         <v>114</v>
       </c>
       <c r="B116">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2002,7 +2149,7 @@
         <v>115</v>
       </c>
       <c r="B117">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2010,7 +2157,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2018,7 +2165,7 @@
         <v>117</v>
       </c>
       <c r="B119">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2026,7 +2173,7 @@
         <v>118</v>
       </c>
       <c r="B120">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -2034,7 +2181,7 @@
         <v>119</v>
       </c>
       <c r="B121">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -2042,7 +2189,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -2050,7 +2197,7 @@
         <v>121</v>
       </c>
       <c r="B123">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -2058,7 +2205,7 @@
         <v>122</v>
       </c>
       <c r="B124">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -2066,7 +2213,7 @@
         <v>123</v>
       </c>
       <c r="B125">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -2074,7 +2221,7 @@
         <v>124</v>
       </c>
       <c r="B126">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -2082,7 +2229,7 @@
         <v>125</v>
       </c>
       <c r="B127">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -2090,7 +2237,7 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -2098,7 +2245,7 @@
         <v>127</v>
       </c>
       <c r="B129">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -2106,7 +2253,7 @@
         <v>128</v>
       </c>
       <c r="B130">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -2114,7 +2261,7 @@
         <v>129</v>
       </c>
       <c r="B131">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -2122,7 +2269,7 @@
         <v>130</v>
       </c>
       <c r="B132">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -2130,7 +2277,7 @@
         <v>131</v>
       </c>
       <c r="B133">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -2138,7 +2285,7 @@
         <v>132</v>
       </c>
       <c r="B134">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -2146,7 +2293,7 @@
         <v>133</v>
       </c>
       <c r="B135">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -2154,7 +2301,7 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2162,7 +2309,7 @@
         <v>135</v>
       </c>
       <c r="B137">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2170,7 +2317,7 @@
         <v>136</v>
       </c>
       <c r="B138">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2178,7 +2325,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2186,7 +2333,7 @@
         <v>138</v>
       </c>
       <c r="B140">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2194,7 +2341,7 @@
         <v>139</v>
       </c>
       <c r="B141">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2202,7 +2349,7 @@
         <v>140</v>
       </c>
       <c r="B142">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2210,7 +2357,7 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -2218,7 +2365,7 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2226,7 +2373,7 @@
         <v>143</v>
       </c>
       <c r="B145">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2234,7 +2381,7 @@
         <v>144</v>
       </c>
       <c r="B146">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2242,7 +2389,7 @@
         <v>145</v>
       </c>
       <c r="B147">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -2250,7 +2397,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2258,7 +2405,7 @@
         <v>147</v>
       </c>
       <c r="B149">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2266,7 +2413,7 @@
         <v>148</v>
       </c>
       <c r="B150">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -2274,7 +2421,7 @@
         <v>149</v>
       </c>
       <c r="B151">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2282,7 +2429,7 @@
         <v>150</v>
       </c>
       <c r="B152">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2290,7 +2437,7 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2298,7 +2445,7 @@
         <v>152</v>
       </c>
       <c r="B154">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2306,7 +2453,7 @@
         <v>153</v>
       </c>
       <c r="B155">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2314,7 +2461,7 @@
         <v>154</v>
       </c>
       <c r="B156">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2322,7 +2469,7 @@
         <v>155</v>
       </c>
       <c r="B157">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2330,7 +2477,7 @@
         <v>156</v>
       </c>
       <c r="B158">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2338,7 +2485,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2346,7 +2493,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2354,7 +2501,7 @@
         <v>159</v>
       </c>
       <c r="B161">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2362,7 +2509,7 @@
         <v>160</v>
       </c>
       <c r="B162">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2370,7 +2517,7 @@
         <v>161</v>
       </c>
       <c r="B163">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2378,7 +2525,7 @@
         <v>162</v>
       </c>
       <c r="B164">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -2386,7 +2533,7 @@
         <v>163</v>
       </c>
       <c r="B165">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -2394,7 +2541,7 @@
         <v>164</v>
       </c>
       <c r="B166">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -2402,7 +2549,7 @@
         <v>165</v>
       </c>
       <c r="B167">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -2410,7 +2557,7 @@
         <v>166</v>
       </c>
       <c r="B168">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -2418,7 +2565,7 @@
         <v>167</v>
       </c>
       <c r="B169">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -2426,7 +2573,7 @@
         <v>168</v>
       </c>
       <c r="B170">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2434,7 +2581,7 @@
         <v>169</v>
       </c>
       <c r="B171">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -2442,7 +2589,7 @@
         <v>170</v>
       </c>
       <c r="B172">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -2450,7 +2597,7 @@
         <v>171</v>
       </c>
       <c r="B173">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -2458,7 +2605,7 @@
         <v>172</v>
       </c>
       <c r="B174">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -2466,7 +2613,7 @@
         <v>173</v>
       </c>
       <c r="B175">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -2474,7 +2621,7 @@
         <v>174</v>
       </c>
       <c r="B176">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -2482,7 +2629,7 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -2490,7 +2637,7 @@
         <v>176</v>
       </c>
       <c r="B178">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -2498,7 +2645,7 @@
         <v>177</v>
       </c>
       <c r="B179">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2506,7 +2653,7 @@
         <v>178</v>
       </c>
       <c r="B180">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -2514,7 +2661,7 @@
         <v>179</v>
       </c>
       <c r="B181">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2522,7 +2669,7 @@
         <v>180</v>
       </c>
       <c r="B182">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -2530,7 +2677,7 @@
         <v>181</v>
       </c>
       <c r="B183">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2538,7 +2685,7 @@
         <v>182</v>
       </c>
       <c r="B184">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -2546,7 +2693,7 @@
         <v>183</v>
       </c>
       <c r="B185">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -2554,7 +2701,7 @@
         <v>184</v>
       </c>
       <c r="B186">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -3010,6 +3157,398 @@
         <v>241</v>
       </c>
       <c r="B243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2">
+      <c r="A244" t="s">
+        <v>242</v>
+      </c>
+      <c r="B244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245" t="s">
+        <v>243</v>
+      </c>
+      <c r="B245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="A246" t="s">
+        <v>244</v>
+      </c>
+      <c r="B246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247" t="s">
+        <v>245</v>
+      </c>
+      <c r="B247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" t="s">
+        <v>246</v>
+      </c>
+      <c r="B248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249" t="s">
+        <v>247</v>
+      </c>
+      <c r="B249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="A250" t="s">
+        <v>248</v>
+      </c>
+      <c r="B250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251" t="s">
+        <v>249</v>
+      </c>
+      <c r="B251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2">
+      <c r="A252" t="s">
+        <v>250</v>
+      </c>
+      <c r="B252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2">
+      <c r="A253" t="s">
+        <v>251</v>
+      </c>
+      <c r="B253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2">
+      <c r="A254" t="s">
+        <v>252</v>
+      </c>
+      <c r="B254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2">
+      <c r="A255" t="s">
+        <v>253</v>
+      </c>
+      <c r="B255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" t="s">
+        <v>254</v>
+      </c>
+      <c r="B256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" t="s">
+        <v>255</v>
+      </c>
+      <c r="B257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" t="s">
+        <v>256</v>
+      </c>
+      <c r="B258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" t="s">
+        <v>257</v>
+      </c>
+      <c r="B259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" t="s">
+        <v>258</v>
+      </c>
+      <c r="B260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261" t="s">
+        <v>259</v>
+      </c>
+      <c r="B261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="A262" t="s">
+        <v>260</v>
+      </c>
+      <c r="B262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="A263" t="s">
+        <v>261</v>
+      </c>
+      <c r="B263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="A264" t="s">
+        <v>262</v>
+      </c>
+      <c r="B264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
+      <c r="A265" t="s">
+        <v>263</v>
+      </c>
+      <c r="B265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
+      <c r="A266" t="s">
+        <v>264</v>
+      </c>
+      <c r="B266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
+      <c r="A267" t="s">
+        <v>265</v>
+      </c>
+      <c r="B267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
+      <c r="A268" t="s">
+        <v>266</v>
+      </c>
+      <c r="B268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
+      <c r="A269" t="s">
+        <v>267</v>
+      </c>
+      <c r="B269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
+      <c r="A270" t="s">
+        <v>268</v>
+      </c>
+      <c r="B270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
+      <c r="A271" t="s">
+        <v>269</v>
+      </c>
+      <c r="B271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2">
+      <c r="A272" t="s">
+        <v>270</v>
+      </c>
+      <c r="B272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2">
+      <c r="A273" t="s">
+        <v>271</v>
+      </c>
+      <c r="B273">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="A274" t="s">
+        <v>272</v>
+      </c>
+      <c r="B274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275" t="s">
+        <v>273</v>
+      </c>
+      <c r="B275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="A276" t="s">
+        <v>274</v>
+      </c>
+      <c r="B276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" t="s">
+        <v>275</v>
+      </c>
+      <c r="B277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2">
+      <c r="A278" t="s">
+        <v>276</v>
+      </c>
+      <c r="B278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2">
+      <c r="A279" t="s">
+        <v>277</v>
+      </c>
+      <c r="B279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2">
+      <c r="A280" t="s">
+        <v>278</v>
+      </c>
+      <c r="B280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2">
+      <c r="A281" t="s">
+        <v>279</v>
+      </c>
+      <c r="B281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2">
+      <c r="A282" t="s">
+        <v>280</v>
+      </c>
+      <c r="B282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2">
+      <c r="A283" t="s">
+        <v>281</v>
+      </c>
+      <c r="B283">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2">
+      <c r="A284" t="s">
+        <v>282</v>
+      </c>
+      <c r="B284">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2">
+      <c r="A285" t="s">
+        <v>283</v>
+      </c>
+      <c r="B285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2">
+      <c r="A286" t="s">
+        <v>284</v>
+      </c>
+      <c r="B286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2">
+      <c r="A287" t="s">
+        <v>285</v>
+      </c>
+      <c r="B287">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2">
+      <c r="A288" t="s">
+        <v>286</v>
+      </c>
+      <c r="B288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2">
+      <c r="A289" t="s">
+        <v>287</v>
+      </c>
+      <c r="B289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2">
+      <c r="A290" t="s">
+        <v>288</v>
+      </c>
+      <c r="B290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2">
+      <c r="A291" t="s">
+        <v>289</v>
+      </c>
+      <c r="B291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2">
+      <c r="A292" t="s">
+        <v>290</v>
+      </c>
+      <c r="B292">
         <v>1</v>
       </c>
     </row>

</xml_diff>